<commit_message>
feat: Update Excel upload endpoint for vendor module and remove profile_picture_url_link from vendorExcelFile
</commit_message>
<xml_diff>
--- a/src/vendorExcelFile.xlsx
+++ b/src/vendorExcelFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\web-dev\fastra-frontend\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0970111C-06AB-44EE-81CD-41730BCB9845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDB59FE-C5C3-462A-B532-BE3F542580ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12060" yWindow="2085" windowWidth="8565" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>company_name</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>phone_number</t>
-  </si>
-  <si>
-    <t>profile_picture_url</t>
   </si>
 </sst>
 </file>
@@ -366,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -377,7 +374,7 @@
     <col min="1" max="6" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -390,9 +387,6 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>